<commit_message>
Fixes for combat multi trauma matrix.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/Showcases/CombatMultitraumaValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/Showcases/CombatMultitraumaValidation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngine\data\human\adult\validation\Scenarios\Showcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F911FAF9-461B-450C-8A55-D74A7E71EA09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E33433-48AE-411A-BA86-2E24AAEB85D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2535" yWindow="345" windowWidth="24825" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="265">
   <si>
     <t>Scenario Overview</t>
   </si>
@@ -1001,15 +1001,6 @@
     <t>A bolus of 5 mg of morphine is administered intravenously. Saline administration continues</t>
   </si>
   <si>
-    <t>A pressure dressing  is applied
-Tension pneumothorax has progressed untreated for 3 minutes.</t>
-  </si>
-  <si>
-    <t>Massive hemorrhage from the right leg.
-350 mL/min
-Tension pneumothorax has progressed untreated for 2 minutes.</t>
-  </si>
-  <si>
     <t>Mean Arterial Pressure  (mmHg)</t>
   </si>
   <si>
@@ -1019,60 +1010,15 @@
     <t>Mean Central Venous Pressure (mmHg)</t>
   </si>
   <si>
-    <t>Respiration Rate
-(Breaths/min)</t>
-  </si>
-  <si>
-    <t>Oxygen Saturation
-(fraction)</t>
-  </si>
-  <si>
-    <t>Tidal Volume
-(mL)</t>
-  </si>
-  <si>
-    <t>~25% Increase@cite gutierrez2004clinical
-Tachycardia @cite leigh2005tension</t>
-  </si>
-  <si>
-    <t>~25% Increase @cite gutierrez2004clinical
-Tachycardia @cite leigh2005tension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NC or decrease @cite leigh2005tension
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">117.9 @cite khorasani2008assessment
- Possibly no significant change @cite price2006novel
-</t>
-  </si>
-  <si>
     <t>15-20% Decrease @cite Morgan2006Clinical</t>
   </si>
   <si>
-    <t xml:space="preserve">Increase @cite grmec2009relationship
-</t>
-  </si>
-  <si>
     <t>Decrease @cite guyton2006medical</t>
   </si>
   <si>
     <t>Increase @cite echt1974effective</t>
   </si>
   <si>
-    <t>Decrease@cite chrisp2000action @cite khorasani2008assessment
-Plateaus @cite waisman2013transient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">~25% Decrease @cite waisman2013transient
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Increase &gt; 0.95 @cite rim2011life
-</t>
-  </si>
-  <si>
     <t>90 - 110 @cite metoyer2016SME</t>
   </si>
   <si>
@@ -1091,32 +1037,12 @@
     <t>Moderate Decrease @cite bergeronSME</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Decrease @cite drummond2010oxygen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-NC or Slight Decrease @cite bergeronSME</t>
-  </si>
-  <si>
-    <t>40 @cite chrisp2000action
-14-20 @cite gutierrez2004clinical
-Tachypnea @cite waisman2013transient @cite army200968w @cite leigh2005tensio</t>
-  </si>
-  <si>
-    <t>Slight decrease because of partial correction of the hypovolemia.@cite metoyer2016SME
-Stress-Induced Moderate Tachycardia @cite bergeronSME</t>
-  </si>
-  <si>
     <t>Decreases @cite guyton2006medical</t>
   </si>
   <si>
     <t>NC @cite guyton2006medical</t>
   </si>
   <si>
-    <t xml:space="preserve">Mild Decrease @cite Morgan2006Clinical      Increase @cite guyton2006medical  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Increase @cite guyton2006medical  </t>
   </si>
   <si>
@@ -1130,6 +1056,161 @@
   </si>
   <si>
     <t>&lt;/span&gt;|</t>
+  </si>
+  <si>
+    <t>Respiration Rate (Breaths/min)</t>
+  </si>
+  <si>
+    <t>Oxygen Saturation (fraction)</t>
+  </si>
+  <si>
+    <t>Tidal Volume (mL)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Begin Tension Pneumothorax </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(Left side, closed, severity 0.75) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Begin Massive Hemorrhage </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Right leg, rate 350 mL/min)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tourniquet </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Hemorrhage completely controlled, rate 0 mL/min)</t>
+    </r>
+  </si>
+  <si>
+    <t>Injuries are untreated.</t>
+  </si>
+  <si>
+    <t>A pressure dressing  is applied.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Intravenous Fluid Resuscitation </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Saline, 500 mL at rate of 100 mL/min)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Narcotics (Morphine) Administration </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(5 mL of morphine IV at concentration of 1 mg/mL)</t>
+    </r>
+  </si>
+  <si>
+    <t>~25% Increase; @cite gutierrez2004clinical Tachycardia @cite leigh2005tension</t>
+  </si>
+  <si>
+    <t>Slight decrease because of partial correction of the hypovolemia; @cite metoyer2016SME Stress-Induced Moderate Tachycardia @cite bergeronSME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mild Decrease; @cite Morgan2006Clinical  Increase @cite guyton2006medical  </t>
+  </si>
+  <si>
+    <t>Decrease; @cite chrisp2000action @cite khorasani2008assessment Plateaus @cite waisman2013transient</t>
+  </si>
+  <si>
+    <t>Decrease @cite drummond2010oxygen</t>
+  </si>
+  <si>
+    <t>NC or decrease @cite leigh2005tension</t>
+  </si>
+  <si>
+    <t>40; @cite chrisp2000action 14-20; @cite gutierrez2004clinical Tachypnea @cite waisman2013transient @cite army200968w @cite leigh2005tension</t>
+  </si>
+  <si>
+    <t>~25% Decrease @cite waisman2013transient</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Non-tourniquet bleeding control </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Manual pressure reduces hemorrhage to 50 mL/min)</t>
+    </r>
+  </si>
+  <si>
+    <t>NC or Slight Decrease @cite bergeronSME</t>
+  </si>
+  <si>
+    <t>Increase &gt; 0.95 @cite rim2011life</t>
+  </si>
+  <si>
+    <t>117.9; @cite khorasani2008assessment Possibly no significant change @cite price2006novel</t>
+  </si>
+  <si>
+    <t>Increase @cite grmec2009relationship</t>
   </si>
 </sst>
 </file>
@@ -1422,7 +1503,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1655,11 +1736,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3419,8 +3512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CEA3A73-A32D-489E-932B-3617BA085B3B}">
   <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+    <sheetView tabSelected="1" topLeftCell="E5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3430,17 +3523,17 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="8" max="8" width="9.85546875" customWidth="1"/>
     <col min="9" max="9" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" customWidth="1"/>
+    <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17" customWidth="1"/>
     <col min="15" max="15" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.85546875" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.5703125" customWidth="1"/>
+    <col min="18" max="18" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19" customWidth="1"/>
+    <col min="20" max="20" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="20.42578125" customWidth="1"/>
   </cols>
@@ -3476,23 +3569,41 @@
       <c r="J1" s="86" t="s">
         <v>220</v>
       </c>
+      <c r="K1" s="84" t="s">
+        <v>215</v>
+      </c>
       <c r="L1" s="86" t="s">
+        <v>224</v>
+      </c>
+      <c r="M1" s="84" t="s">
+        <v>215</v>
+      </c>
+      <c r="N1" s="86" t="s">
+        <v>225</v>
+      </c>
+      <c r="O1" s="84" t="s">
+        <v>215</v>
+      </c>
+      <c r="P1" s="86" t="s">
         <v>226</v>
       </c>
-      <c r="N1" s="86" t="s">
-        <v>227</v>
-      </c>
-      <c r="P1" s="86" t="s">
-        <v>228</v>
-      </c>
-      <c r="R1" s="32" t="s">
-        <v>229</v>
-      </c>
-      <c r="T1" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="V1" s="32" t="s">
-        <v>231</v>
+      <c r="Q1" s="84" t="s">
+        <v>215</v>
+      </c>
+      <c r="R1" s="89" t="s">
+        <v>243</v>
+      </c>
+      <c r="S1" s="84" t="s">
+        <v>215</v>
+      </c>
+      <c r="T1" s="89" t="s">
+        <v>244</v>
+      </c>
+      <c r="U1" s="84" t="s">
+        <v>215</v>
+      </c>
+      <c r="V1" s="89" t="s">
+        <v>245</v>
       </c>
       <c r="W1" s="84" t="s">
         <v>215</v>
@@ -3517,8 +3628,8 @@
       <c r="F2" s="84" t="s">
         <v>215</v>
       </c>
-      <c r="G2" s="87" t="s">
-        <v>221</v>
+      <c r="G2" s="84" t="s">
+        <v>215</v>
       </c>
       <c r="H2" s="87" t="s">
         <v>221</v>
@@ -3573,14 +3684,14 @@
       <c r="A3" s="84" t="s">
         <v>215</v>
       </c>
-      <c r="B3" s="38" t="s">
-        <v>102</v>
+      <c r="B3" s="90" t="s">
+        <v>246</v>
       </c>
       <c r="C3" s="84" t="s">
         <v>215</v>
       </c>
-      <c r="D3" s="38" t="s">
-        <v>225</v>
+      <c r="D3" s="90" t="s">
+        <v>248</v>
       </c>
       <c r="E3" s="84" t="s">
         <v>215</v>
@@ -3595,63 +3706,63 @@
         <v>120</v>
       </c>
       <c r="I3" s="84" t="s">
+        <v>240</v>
+      </c>
+      <c r="J3" s="91" t="s">
+        <v>252</v>
+      </c>
+      <c r="K3" s="84" t="s">
+        <v>240</v>
+      </c>
+      <c r="L3" s="91" t="s">
+        <v>257</v>
+      </c>
+      <c r="M3" s="84" t="s">
+        <v>240</v>
+      </c>
+      <c r="N3" s="91" t="s">
+        <v>228</v>
+      </c>
+      <c r="O3" s="84" t="s">
+        <v>240</v>
+      </c>
+      <c r="P3" s="91" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q3" s="84" t="s">
+        <v>240</v>
+      </c>
+      <c r="R3" s="91" t="s">
         <v>258</v>
       </c>
-      <c r="J3" s="40" t="s">
-        <v>232</v>
-      </c>
-      <c r="K3" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="L3" s="40" t="s">
-        <v>234</v>
-      </c>
-      <c r="M3" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="N3" s="40" t="s">
-        <v>238</v>
-      </c>
-      <c r="O3" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="P3" s="40" t="s">
+      <c r="S3" s="84" t="s">
+        <v>240</v>
+      </c>
+      <c r="T3" s="91" t="s">
         <v>239</v>
       </c>
-      <c r="Q3" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="R3" s="40" t="s">
-        <v>251</v>
-      </c>
-      <c r="S3" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="T3" s="40" t="s">
-        <v>257</v>
-      </c>
       <c r="U3" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="V3" s="40" t="s">
-        <v>241</v>
+        <v>240</v>
+      </c>
+      <c r="V3" s="91" t="s">
+        <v>259</v>
       </c>
       <c r="W3" s="84" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="84" t="s">
         <v>215</v>
       </c>
-      <c r="B4" s="30" t="s">
-        <v>103</v>
+      <c r="B4" s="87" t="s">
+        <v>260</v>
       </c>
       <c r="C4" s="84" t="s">
         <v>215</v>
       </c>
-      <c r="D4" s="38" t="s">
-        <v>224</v>
+      <c r="D4" s="90" t="s">
+        <v>249</v>
       </c>
       <c r="E4" s="84" t="s">
         <v>215</v>
@@ -3666,62 +3777,62 @@
         <v>180</v>
       </c>
       <c r="I4" s="84" t="s">
+        <v>240</v>
+      </c>
+      <c r="J4" s="91" t="s">
+        <v>252</v>
+      </c>
+      <c r="K4" s="84" t="s">
+        <v>240</v>
+      </c>
+      <c r="L4" s="91" t="s">
+        <v>257</v>
+      </c>
+      <c r="M4" s="84" t="s">
+        <v>240</v>
+      </c>
+      <c r="N4" s="91" t="s">
+        <v>228</v>
+      </c>
+      <c r="O4" s="84" t="s">
+        <v>240</v>
+      </c>
+      <c r="P4" s="91" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q4" s="84" t="s">
+        <v>240</v>
+      </c>
+      <c r="R4" s="91" t="s">
         <v>258</v>
       </c>
-      <c r="J4" s="40" t="s">
-        <v>233</v>
-      </c>
-      <c r="K4" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="L4" s="40" t="s">
-        <v>234</v>
-      </c>
-      <c r="M4" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="N4" s="40" t="s">
-        <v>238</v>
-      </c>
-      <c r="O4" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="P4" s="40" t="s">
-        <v>239</v>
-      </c>
-      <c r="Q4" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="R4" s="40" t="s">
-        <v>251</v>
-      </c>
       <c r="S4" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="T4" s="40" t="s">
         <v>240</v>
       </c>
+      <c r="T4" s="91" t="s">
+        <v>255</v>
+      </c>
       <c r="U4" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="V4" s="40" t="s">
-        <v>241</v>
+        <v>240</v>
+      </c>
+      <c r="V4" s="91" t="s">
+        <v>259</v>
       </c>
       <c r="W4" s="84" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="84" t="s">
         <v>215</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="87" t="s">
         <v>104</v>
       </c>
       <c r="C5" s="84" t="s">
         <v>215</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="90" t="s">
         <v>50</v>
       </c>
       <c r="E5" s="84" t="s">
@@ -3737,62 +3848,62 @@
         <v>420</v>
       </c>
       <c r="I5" s="84" t="s">
-        <v>259</v>
-      </c>
-      <c r="J5" s="41" t="s">
-        <v>243</v>
+        <v>241</v>
+      </c>
+      <c r="J5" s="92" t="s">
+        <v>230</v>
       </c>
       <c r="K5" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="L5" s="40" t="s">
-        <v>253</v>
+        <v>240</v>
+      </c>
+      <c r="L5" s="91" t="s">
+        <v>236</v>
       </c>
       <c r="M5" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="N5" s="40" t="s">
-        <v>238</v>
+        <v>240</v>
+      </c>
+      <c r="N5" s="91" t="s">
+        <v>228</v>
       </c>
       <c r="O5" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="P5" s="40" t="s">
-        <v>250</v>
+        <v>240</v>
+      </c>
+      <c r="P5" s="91" t="s">
+        <v>261</v>
       </c>
       <c r="Q5" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="R5" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="R5" s="91" t="s">
+        <v>234</v>
+      </c>
+      <c r="S5" s="84" t="s">
+        <v>240</v>
+      </c>
+      <c r="T5" s="91" t="s">
+        <v>262</v>
+      </c>
+      <c r="U5" s="84" t="s">
+        <v>240</v>
+      </c>
+      <c r="V5" s="91" t="s">
+        <v>234</v>
+      </c>
+      <c r="W5" s="84" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="84" t="s">
+        <v>215</v>
+      </c>
+      <c r="B6" s="87" t="s">
         <v>247</v>
       </c>
-      <c r="S5" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="T5" s="40" t="s">
-        <v>242</v>
-      </c>
-      <c r="U5" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="V5" s="40" t="s">
-        <v>247</v>
-      </c>
-      <c r="W5" s="84" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="84" t="s">
-        <v>215</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>105</v>
-      </c>
       <c r="C6" s="84" t="s">
         <v>215</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="90" t="s">
         <v>222</v>
       </c>
       <c r="E6" s="84" t="s">
@@ -3808,62 +3919,62 @@
         <v>450</v>
       </c>
       <c r="I6" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="J6" s="40" t="s">
-        <v>235</v>
+        <v>240</v>
+      </c>
+      <c r="J6" s="91" t="s">
+        <v>263</v>
       </c>
       <c r="K6" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="L6" s="40" t="s">
-        <v>254</v>
+        <v>240</v>
+      </c>
+      <c r="L6" s="91" t="s">
+        <v>237</v>
       </c>
       <c r="M6" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="N6" s="40" t="s">
-        <v>254</v>
+        <v>240</v>
+      </c>
+      <c r="N6" s="91" t="s">
+        <v>237</v>
       </c>
       <c r="O6" s="84" t="s">
-        <v>259</v>
-      </c>
-      <c r="P6" s="41" t="s">
-        <v>250</v>
+        <v>241</v>
+      </c>
+      <c r="P6" s="92" t="s">
+        <v>261</v>
       </c>
       <c r="Q6" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="R6" s="40" t="s">
-        <v>247</v>
+        <v>240</v>
+      </c>
+      <c r="R6" s="91" t="s">
+        <v>234</v>
       </c>
       <c r="S6" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="T6" s="40" t="s">
-        <v>247</v>
+        <v>240</v>
+      </c>
+      <c r="T6" s="91" t="s">
+        <v>234</v>
       </c>
       <c r="U6" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="V6" s="40" t="s">
-        <v>247</v>
+        <v>240</v>
+      </c>
+      <c r="V6" s="91" t="s">
+        <v>234</v>
       </c>
       <c r="W6" s="84" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="84" t="s">
         <v>215</v>
       </c>
-      <c r="B7" s="30" t="s">
-        <v>106</v>
+      <c r="B7" s="87" t="s">
+        <v>250</v>
       </c>
       <c r="C7" s="84" t="s">
         <v>215</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="90" t="s">
         <v>54</v>
       </c>
       <c r="E7" s="84" t="s">
@@ -3879,62 +3990,62 @@
         <v>570</v>
       </c>
       <c r="I7" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="J7" s="40" t="s">
-        <v>252</v>
+        <v>240</v>
+      </c>
+      <c r="J7" s="91" t="s">
+        <v>253</v>
       </c>
       <c r="K7" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="L7" s="40" t="s">
-        <v>237</v>
+        <v>240</v>
+      </c>
+      <c r="L7" s="91" t="s">
+        <v>264</v>
       </c>
       <c r="M7" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="N7" s="40" t="s">
-        <v>256</v>
+        <v>240</v>
+      </c>
+      <c r="N7" s="91" t="s">
+        <v>238</v>
       </c>
       <c r="O7" s="84" t="s">
-        <v>259</v>
-      </c>
-      <c r="P7" s="41" t="s">
-        <v>245</v>
+        <v>241</v>
+      </c>
+      <c r="P7" s="92" t="s">
+        <v>232</v>
       </c>
       <c r="Q7" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="R7" s="40" t="s">
-        <v>247</v>
+        <v>240</v>
+      </c>
+      <c r="R7" s="91" t="s">
+        <v>234</v>
       </c>
       <c r="S7" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="T7" s="40" t="s">
-        <v>247</v>
+        <v>240</v>
+      </c>
+      <c r="T7" s="91" t="s">
+        <v>234</v>
       </c>
       <c r="U7" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="V7" s="40" t="s">
-        <v>247</v>
+        <v>240</v>
+      </c>
+      <c r="V7" s="91" t="s">
+        <v>234</v>
       </c>
       <c r="W7" s="84" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="84" t="s">
         <v>215</v>
       </c>
-      <c r="B8" s="30" t="s">
-        <v>107</v>
+      <c r="B8" s="87" t="s">
+        <v>251</v>
       </c>
       <c r="C8" s="84" t="s">
         <v>215</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="90" t="s">
         <v>223</v>
       </c>
       <c r="E8" s="84" t="s">
@@ -3950,53 +4061,53 @@
         <v>730</v>
       </c>
       <c r="I8" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="J8" s="88" t="s">
-        <v>244</v>
+        <v>240</v>
+      </c>
+      <c r="J8" s="93" t="s">
+        <v>231</v>
       </c>
       <c r="K8" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="L8" s="88" t="s">
-        <v>255</v>
+        <v>240</v>
+      </c>
+      <c r="L8" s="93" t="s">
+        <v>254</v>
       </c>
       <c r="M8" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="N8" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="N8" s="91" t="s">
+        <v>238</v>
+      </c>
+      <c r="O8" s="84" t="s">
+        <v>240</v>
+      </c>
+      <c r="P8" s="91" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q8" s="84" t="s">
+        <v>240</v>
+      </c>
+      <c r="R8" s="93" t="s">
+        <v>227</v>
+      </c>
+      <c r="S8" s="84" t="s">
+        <v>240</v>
+      </c>
+      <c r="T8" s="91" t="s">
         <v>256</v>
       </c>
-      <c r="O8" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="P8" s="40" t="s">
-        <v>246</v>
-      </c>
-      <c r="Q8" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="R8" s="88" t="s">
-        <v>236</v>
-      </c>
-      <c r="S8" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="T8" s="40" t="s">
-        <v>249</v>
-      </c>
       <c r="U8" s="84" t="s">
-        <v>259</v>
-      </c>
-      <c r="V8" s="41" t="s">
-        <v>248</v>
+        <v>241</v>
+      </c>
+      <c r="V8" s="92" t="s">
+        <v>235</v>
       </c>
       <c r="W8" s="84" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L9" s="89"/>
+      <c r="L9" s="88"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixing the color coding.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/Showcases/CombatMultitraumaValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/Showcases/CombatMultitraumaValidation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngine\data\human\adult\validation\Scenarios\Showcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400B3165-E82C-40D1-A341-DC56CCB4F7B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0D87D3-27D0-422B-8A66-909916946E34}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="24825" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="265">
   <si>
     <t>Scenario Overview</t>
   </si>
@@ -1047,9 +1047,6 @@
   </si>
   <si>
     <t>Decrease @cite chrisp2000action @cite army200968w @cite leigh2005tension @cite khorasani2008assessment</t>
-  </si>
-  <si>
-    <t>|&lt;span class="success"&gt;</t>
   </si>
   <si>
     <t>&lt;/span&gt;|</t>
@@ -3519,7 +3516,7 @@
   <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W8" sqref="A1:W8"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3597,19 +3594,19 @@
         <v>215</v>
       </c>
       <c r="R1" s="76" t="s">
+        <v>241</v>
+      </c>
+      <c r="S1" s="71" t="s">
+        <v>215</v>
+      </c>
+      <c r="T1" s="76" t="s">
         <v>242</v>
       </c>
-      <c r="S1" s="71" t="s">
-        <v>215</v>
-      </c>
-      <c r="T1" s="76" t="s">
+      <c r="U1" s="71" t="s">
+        <v>215</v>
+      </c>
+      <c r="V1" s="76" t="s">
         <v>243</v>
-      </c>
-      <c r="U1" s="71" t="s">
-        <v>215</v>
-      </c>
-      <c r="V1" s="76" t="s">
-        <v>244</v>
       </c>
       <c r="W1" s="71" t="s">
         <v>215</v>
@@ -3691,13 +3688,13 @@
         <v>215</v>
       </c>
       <c r="B3" s="77" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C3" s="71" t="s">
         <v>215</v>
       </c>
       <c r="D3" s="77" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E3" s="71" t="s">
         <v>215</v>
@@ -3712,49 +3709,49 @@
         <v>120</v>
       </c>
       <c r="I3" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J3" s="78" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K3" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L3" s="78" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M3" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N3" s="78" t="s">
         <v>228</v>
       </c>
       <c r="O3" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="P3" s="78" t="s">
         <v>229</v>
       </c>
       <c r="Q3" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="R3" s="78" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="S3" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="T3" s="78" t="s">
         <v>239</v>
       </c>
       <c r="U3" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V3" s="78" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="W3" s="71" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="135" x14ac:dyDescent="0.25">
@@ -3762,13 +3759,13 @@
         <v>215</v>
       </c>
       <c r="B4" s="74" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C4" s="71" t="s">
         <v>215</v>
       </c>
       <c r="D4" s="77" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E4" s="71" t="s">
         <v>215</v>
@@ -3783,49 +3780,49 @@
         <v>180</v>
       </c>
       <c r="I4" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J4" s="78" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K4" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L4" s="78" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M4" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N4" s="78" t="s">
         <v>228</v>
       </c>
       <c r="O4" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="P4" s="78" t="s">
         <v>229</v>
       </c>
       <c r="Q4" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="R4" s="78" t="s">
+        <v>256</v>
+      </c>
+      <c r="S4" s="94" t="s">
+        <v>263</v>
+      </c>
+      <c r="T4" s="78" t="s">
+        <v>253</v>
+      </c>
+      <c r="U4" s="94" t="s">
+        <v>263</v>
+      </c>
+      <c r="V4" s="78" t="s">
         <v>257</v>
       </c>
-      <c r="S4" s="94" t="s">
-        <v>264</v>
-      </c>
-      <c r="T4" s="78" t="s">
-        <v>254</v>
-      </c>
-      <c r="U4" s="94" t="s">
-        <v>264</v>
-      </c>
-      <c r="V4" s="78" t="s">
-        <v>258</v>
-      </c>
       <c r="W4" s="71" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -3854,49 +3851,49 @@
         <v>420</v>
       </c>
       <c r="I5" s="94" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J5" s="79" t="s">
         <v>230</v>
       </c>
-      <c r="K5" s="71" t="s">
-        <v>240</v>
+      <c r="K5" s="94" t="s">
+        <v>263</v>
       </c>
       <c r="L5" s="78" t="s">
         <v>236</v>
       </c>
       <c r="M5" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N5" s="78" t="s">
         <v>228</v>
       </c>
       <c r="O5" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="P5" s="78" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Q5" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="R5" s="78" t="s">
         <v>234</v>
       </c>
       <c r="S5" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="T5" s="78" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="U5" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V5" s="78" t="s">
         <v>234</v>
       </c>
       <c r="W5" s="71" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="75" x14ac:dyDescent="0.25">
@@ -3904,7 +3901,7 @@
         <v>215</v>
       </c>
       <c r="B6" s="74" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C6" s="71" t="s">
         <v>215</v>
@@ -3925,49 +3922,49 @@
         <v>450</v>
       </c>
       <c r="I6" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J6" s="78" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K6" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L6" s="78" t="s">
         <v>237</v>
       </c>
       <c r="M6" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N6" s="78" t="s">
         <v>237</v>
       </c>
       <c r="O6" s="94" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="P6" s="79" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Q6" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="R6" s="78" t="s">
         <v>234</v>
       </c>
       <c r="S6" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="T6" s="78" t="s">
         <v>234</v>
       </c>
       <c r="U6" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V6" s="78" t="s">
         <v>234</v>
       </c>
       <c r="W6" s="71" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="105" x14ac:dyDescent="0.25">
@@ -3975,7 +3972,7 @@
         <v>215</v>
       </c>
       <c r="B7" s="74" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C7" s="71" t="s">
         <v>215</v>
@@ -3996,49 +3993,49 @@
         <v>570</v>
       </c>
       <c r="I7" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J7" s="78" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K7" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L7" s="78" t="s">
+        <v>262</v>
+      </c>
+      <c r="M7" s="94" t="s">
         <v>263</v>
-      </c>
-      <c r="M7" s="94" t="s">
-        <v>264</v>
       </c>
       <c r="N7" s="78" t="s">
         <v>238</v>
       </c>
       <c r="O7" s="94" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="P7" s="79" t="s">
         <v>232</v>
       </c>
       <c r="Q7" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="R7" s="78" t="s">
         <v>234</v>
       </c>
       <c r="S7" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="T7" s="78" t="s">
         <v>234</v>
       </c>
       <c r="U7" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V7" s="78" t="s">
         <v>234</v>
       </c>
       <c r="W7" s="71" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="60" x14ac:dyDescent="0.25">
@@ -4046,7 +4043,7 @@
         <v>215</v>
       </c>
       <c r="B8" s="74" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C8" s="71" t="s">
         <v>215</v>
@@ -4067,49 +4064,49 @@
         <v>730</v>
       </c>
       <c r="I8" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J8" s="80" t="s">
         <v>231</v>
       </c>
       <c r="K8" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L8" s="80" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M8" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N8" s="78" t="s">
         <v>238</v>
       </c>
       <c r="O8" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="P8" s="78" t="s">
         <v>233</v>
       </c>
       <c r="Q8" s="94" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="R8" s="80" t="s">
         <v>227</v>
       </c>
       <c r="S8" s="94" t="s">
+        <v>263</v>
+      </c>
+      <c r="T8" s="78" t="s">
+        <v>254</v>
+      </c>
+      <c r="U8" s="94" t="s">
         <v>264</v>
-      </c>
-      <c r="T8" s="78" t="s">
-        <v>255</v>
-      </c>
-      <c r="U8" s="94" t="s">
-        <v>265</v>
       </c>
       <c r="V8" s="79" t="s">
         <v>235</v>
       </c>
       <c r="W8" s="71" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>